<commit_message>
Good shot with pic
</commit_message>
<xml_diff>
--- a/Ideal_gas/Properties.xlsx
+++ b/Ideal_gas/Properties.xlsx
@@ -467,13 +467,13 @@
         <v>0.415592138226142</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5672518014907837</v>
+        <v>0.5713659524917603</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1516596632646417</v>
+        <v>0.1557738142656183</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3649242834861255</v>
+        <v>0.3748237753738615</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         <v>0.494042374708121</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6810336709022522</v>
+        <v>0.6845132112503052</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1869912961941312</v>
+        <v>0.1904708365421842</v>
       </c>
       <c r="E3" t="n">
-        <v>0.378492424469875</v>
+        <v>0.3855354242735026</v>
       </c>
     </row>
     <row r="4">
@@ -501,13 +501,13 @@
         <v>0.513501221426955</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7152469158172607</v>
+        <v>0.7185081243515015</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2017456943903058</v>
+        <v>0.2050069029245465</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3928825988566882</v>
+        <v>0.3992335253942692</v>
       </c>
     </row>
     <row r="5">
@@ -518,13 +518,13 @@
         <v>0.519870870623062</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1967882513999939</v>
+        <v>0.2049598693847656</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3230826192230681</v>
+        <v>0.3149110012382964</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6214670555321855</v>
+        <v>0.6057485022403304</v>
       </c>
     </row>
     <row r="6">
@@ -535,13 +535,13 @@
         <v>0.6956893984677111</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7172962427139282</v>
+        <v>0.7216441631317139</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02160684424621717</v>
+        <v>0.02595476466400282</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03105817667166881</v>
+        <v>0.03730797784351669</v>
       </c>
     </row>
     <row r="7">
@@ -552,13 +552,13 @@
         <v>0.929780442305243</v>
       </c>
       <c r="C7" t="n">
-        <v>0.703768253326416</v>
+        <v>0.7104123830795288</v>
       </c>
       <c r="D7" t="n">
-        <v>0.226012188978827</v>
+        <v>0.2193680592257142</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2430812465988913</v>
+        <v>0.2359353340255533</v>
       </c>
     </row>
     <row r="8">
@@ -569,13 +569,13 @@
         <v>0.941113649257159</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7568719387054443</v>
+        <v>0.7629913091659546</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1842417105517147</v>
+        <v>0.1781223400912044</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1957698846437309</v>
+        <v>0.1892676195184292</v>
       </c>
     </row>
     <row r="9">
@@ -586,13 +586,13 @@
         <v>0.956562860016915</v>
       </c>
       <c r="C9" t="n">
-        <v>1.031036496162415</v>
+        <v>1.033882260322571</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07447363614549951</v>
+        <v>0.07731940030565576</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0778554544174782</v>
+        <v>0.08083044359916766</v>
       </c>
     </row>
     <row r="10">
@@ -603,13 +603,13 @@
         <v>0.959164174307957</v>
       </c>
       <c r="C10" t="n">
-        <v>1.124603152275085</v>
+        <v>1.126290202140808</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1654389779671285</v>
+        <v>0.1671260278328511</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1724824408568989</v>
+        <v>0.1742413158346262</v>
       </c>
     </row>
     <row r="11">
@@ -620,13 +620,13 @@
         <v>0.9833049531731139</v>
       </c>
       <c r="C11" t="n">
-        <v>1.010159850120544</v>
+        <v>1.013521313667297</v>
       </c>
       <c r="D11" t="n">
-        <v>0.02685489694743048</v>
+        <v>0.03021636049418341</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02731085291574098</v>
+        <v>0.03072938908390074</v>
       </c>
     </row>
     <row r="12">
@@ -637,13 +637,13 @@
         <v>1.13646578692571</v>
       </c>
       <c r="C12" t="n">
-        <v>1.049288630485535</v>
+        <v>1.053916335105896</v>
       </c>
       <c r="D12" t="n">
-        <v>0.08717715644017532</v>
+        <v>0.08254945181981399</v>
       </c>
       <c r="E12" t="n">
-        <v>0.076709002103795</v>
+        <v>0.07263698808137564</v>
       </c>
     </row>
     <row r="13">
@@ -654,13 +654,13 @@
         <v>1.1564261001094</v>
       </c>
       <c r="C13" t="n">
-        <v>1.1415696144104</v>
+        <v>1.145054697990417</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01485648569899967</v>
+        <v>0.01137140211898258</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01284689587825302</v>
+        <v>0.0098332285287463</v>
       </c>
     </row>
     <row r="14">
@@ -671,13 +671,13 @@
         <v>1.19703587214665</v>
       </c>
       <c r="C14" t="n">
-        <v>1.355875492095947</v>
+        <v>1.356420040130615</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1588396199492972</v>
+        <v>0.1593841679839652</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1326941185684347</v>
+        <v>0.1331490322826673</v>
       </c>
     </row>
     <row r="15">
@@ -688,13 +688,13 @@
         <v>1.1986817221463</v>
       </c>
       <c r="C15" t="n">
-        <v>1.135959148406982</v>
+        <v>1.140150547027588</v>
       </c>
       <c r="D15" t="n">
-        <v>0.06272257373931756</v>
+        <v>0.05853117511871209</v>
       </c>
       <c r="E15" t="n">
-        <v>0.05232629527962571</v>
+        <v>0.04882962177308341</v>
       </c>
     </row>
     <row r="16">
@@ -705,13 +705,13 @@
         <v>1.22090612611727</v>
       </c>
       <c r="C16" t="n">
-        <v>1.186826705932617</v>
+        <v>1.190515637397766</v>
       </c>
       <c r="D16" t="n">
-        <v>0.03407942018465282</v>
+        <v>0.03039048871950389</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02791321908837685</v>
+        <v>0.02489174889813342</v>
       </c>
     </row>
     <row r="17">
@@ -722,13 +722,13 @@
         <v>1.4448575566706</v>
       </c>
       <c r="C17" t="n">
-        <v>1.478122353553772</v>
+        <v>1.480097651481628</v>
       </c>
       <c r="D17" t="n">
-        <v>0.03326479688317208</v>
+        <v>0.03524009481102852</v>
       </c>
       <c r="E17" t="n">
-        <v>0.02302289020090291</v>
+        <v>0.02439001315273779</v>
       </c>
     </row>
     <row r="18">
@@ -739,13 +739,13 @@
         <v>1.60134238576435</v>
       </c>
       <c r="C18" t="n">
-        <v>1.611536502838135</v>
+        <v>1.614594459533691</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0101941170737847</v>
+        <v>0.01325207376934134</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00636598216871582</v>
+        <v>0.008275602948594835</v>
       </c>
     </row>
     <row r="19">
@@ -756,13 +756,13 @@
         <v>1.72718902069298</v>
       </c>
       <c r="C19" t="n">
-        <v>1.786407470703125</v>
+        <v>1.786156296730042</v>
       </c>
       <c r="D19" t="n">
-        <v>0.05921845001014492</v>
+        <v>0.05896727603706142</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03428602735465826</v>
+        <v>0.03414060379645226</v>
       </c>
     </row>
     <row r="20">
@@ -773,13 +773,13 @@
         <v>1.88414968409158</v>
       </c>
       <c r="C20" t="n">
-        <v>1.921823024749756</v>
+        <v>1.920592665672302</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03767334065817596</v>
+        <v>0.03644298158072234</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01999487672145311</v>
+        <v>0.01934187176763129</v>
       </c>
     </row>
     <row r="21">
@@ -790,13 +790,13 @@
         <v>2.02594757687927</v>
       </c>
       <c r="C21" t="n">
-        <v>2.067370891571045</v>
+        <v>2.066346883773804</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04142331469177485</v>
+        <v>0.04039930689453364</v>
       </c>
       <c r="E21" t="n">
-        <v>0.02044639020501336</v>
+        <v>0.01994094386033618</v>
       </c>
     </row>
     <row r="22">
@@ -807,13 +807,13 @@
         <v>2.10742967874011</v>
       </c>
       <c r="C22" t="n">
-        <v>2.181900978088379</v>
+        <v>2.181281328201294</v>
       </c>
       <c r="D22" t="n">
-        <v>0.07447129934826879</v>
+        <v>0.07385164946118383</v>
       </c>
       <c r="E22" t="n">
-        <v>0.03533750145949836</v>
+        <v>0.03504347034978398</v>
       </c>
     </row>
     <row r="23">
@@ -824,13 +824,13 @@
         <v>2.34298236626143</v>
       </c>
       <c r="C23" t="n">
-        <v>2.433157682418823</v>
+        <v>2.431698560714722</v>
       </c>
       <c r="D23" t="n">
-        <v>0.09017531615739305</v>
+        <v>0.08871619445329149</v>
       </c>
       <c r="E23" t="n">
-        <v>0.03848740709955957</v>
+        <v>0.03786464453629291</v>
       </c>
     </row>
     <row r="24">
@@ -841,13 +841,13 @@
         <v>2.426543304915</v>
       </c>
       <c r="C24" t="n">
-        <v>2.443727016448975</v>
+        <v>2.441366672515869</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01718371153397458</v>
+        <v>0.01482336760086911</v>
       </c>
       <c r="E24" t="n">
-        <v>0.007081559805328308</v>
+        <v>0.006108841153110334</v>
       </c>
     </row>
     <row r="25">
@@ -858,13 +858,13 @@
         <v>2.47130339805696</v>
       </c>
       <c r="C25" t="n">
-        <v>2.561439752578735</v>
+        <v>2.559452772140503</v>
       </c>
       <c r="D25" t="n">
-        <v>0.09013635452177526</v>
+        <v>0.08814937408354284</v>
       </c>
       <c r="E25" t="n">
-        <v>0.03647320462256644</v>
+        <v>0.03566918337620929</v>
       </c>
     </row>
     <row r="26">
@@ -875,13 +875,13 @@
         <v>2.72144819651732</v>
       </c>
       <c r="C26" t="n">
-        <v>2.985017776489258</v>
+        <v>2.982788801193237</v>
       </c>
       <c r="D26" t="n">
-        <v>0.263569579971938</v>
+        <v>0.2613406046759175</v>
       </c>
       <c r="E26" t="n">
-        <v>0.09684901601626374</v>
+        <v>0.09602997588209071</v>
       </c>
     </row>
     <row r="27">
@@ -892,13 +892,13 @@
         <v>2.73876497306704</v>
       </c>
       <c r="C27" t="n">
-        <v>2.685037136077881</v>
+        <v>2.681436061859131</v>
       </c>
       <c r="D27" t="n">
-        <v>0.05372783698915917</v>
+        <v>0.05732891120790917</v>
       </c>
       <c r="E27" t="n">
-        <v>0.01961754203720204</v>
+        <v>0.02093239535764498</v>
       </c>
     </row>
     <row r="28">
@@ -909,13 +909,13 @@
         <v>3.02403183192847</v>
       </c>
       <c r="C28" t="n">
-        <v>3.18571949005127</v>
+        <v>3.181811332702637</v>
       </c>
       <c r="D28" t="n">
-        <v>0.1616876581227995</v>
+        <v>0.1577795007741667</v>
       </c>
       <c r="E28" t="n">
-        <v>0.05346757809083275</v>
+        <v>0.05217521161923364</v>
       </c>
     </row>
     <row r="29">
@@ -926,13 +926,13 @@
         <v>3.08846720385103</v>
       </c>
       <c r="C29" t="n">
-        <v>3.151129007339478</v>
+        <v>3.146762371063232</v>
       </c>
       <c r="D29" t="n">
-        <v>0.06266180348844763</v>
+        <v>0.05829516721220251</v>
       </c>
       <c r="E29" t="n">
-        <v>0.02028896515731629</v>
+        <v>0.01887511291669663</v>
       </c>
     </row>
     <row r="30">
@@ -943,13 +943,13 @@
         <v>3.36523459549796</v>
       </c>
       <c r="C30" t="n">
-        <v>3.349588632583618</v>
+        <v>3.344161987304688</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01564596291434173</v>
+        <v>0.02107260819327239</v>
       </c>
       <c r="E30" t="n">
-        <v>0.004649293376239812</v>
+        <v>0.006261854142787997</v>
       </c>
     </row>
     <row r="31">
@@ -960,13 +960,13 @@
         <v>3.79659611739957</v>
       </c>
       <c r="C31" t="n">
-        <v>3.613967180252075</v>
+        <v>3.60708212852478</v>
       </c>
       <c r="D31" t="n">
-        <v>0.182628937147495</v>
+        <v>0.1895139888747899</v>
       </c>
       <c r="E31" t="n">
-        <v>0.04810333559330095</v>
+        <v>0.04991681575141974</v>
       </c>
     </row>
   </sheetData>
@@ -1105,8 +1105,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[[-0.5728144   0.60612434  0.18236317 -0.5274476 ]
- [ 0.5304967  -0.01782386 -0.45773685 -0.13646808]]</t>
+          <t>[[ 0.66366774 -0.9729913  -0.24840993 -0.1595111 ]
+ [ 0.23772676  0.34955534 -0.893001    0.6390084 ]]</t>
         </is>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[ 0.04482487 -0.14515175  0.38232458 -0.7213727 ]</t>
+          <t>[-0.24670653 -0.5676868   0.09387612  0.44947824]</t>
         </is>
       </c>
     </row>
@@ -1126,10 +1126,10 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[[-0.34404925]
- [ 0.14738537]
- [ 0.62514174]
- [-1.0843369 ]]</t>
+          <t>[[-0.4445369 ]
+ [-1.5149025 ]
+ [ 0.27909163]
+ [ 0.88200885]]</t>
         </is>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[0.86807805]</t>
+          <t>[0.4606782]</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1174,7 +1174,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.091073902329241</v>
+        <v>2.012052578680841</v>
       </c>
     </row>
     <row r="3">
@@ -1182,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2.081583801627853</v>
+        <v>2.007763220037561</v>
       </c>
     </row>
     <row r="4">
@@ -1190,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2.072485017802863</v>
+        <v>1.996581673009872</v>
       </c>
     </row>
     <row r="5">
@@ -1198,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2.064840780220682</v>
+        <v>1.985051617948153</v>
       </c>
     </row>
     <row r="6">
@@ -1206,7 +1206,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2.058489281104559</v>
+        <v>1.972624281822496</v>
       </c>
     </row>
     <row r="7">
@@ -1214,7 +1214,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2.053103108049846</v>
+        <v>1.955526843486354</v>
       </c>
     </row>
     <row r="8">
@@ -1222,7 +1222,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2.04859653905941</v>
+        <v>1.94028297641464</v>
       </c>
     </row>
     <row r="9">
@@ -1230,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.044888529829015</v>
+        <v>1.924651830323799</v>
       </c>
     </row>
     <row r="10">
@@ -1238,7 +1238,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2.04091983552133</v>
+        <v>1.910739676965092</v>
       </c>
     </row>
     <row r="11">
@@ -1246,7 +1246,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>2.03768909723604</v>
+        <v>1.894927999895082</v>
       </c>
     </row>
     <row r="12">
@@ -1254,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2.034408226855194</v>
+        <v>1.873504996336604</v>
       </c>
     </row>
     <row r="13">
@@ -1262,7 +1262,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>2.031945094973788</v>
+        <v>1.854100351183536</v>
       </c>
     </row>
     <row r="14">
@@ -1270,7 +1270,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2.029027809023938</v>
+        <v>1.817773907051587</v>
       </c>
     </row>
     <row r="15">
@@ -1278,7 +1278,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2.026889757543167</v>
+        <v>1.753624092634226</v>
       </c>
     </row>
     <row r="16">
@@ -1286,7 +1286,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.02480844133231</v>
+        <v>1.580902299611636</v>
       </c>
     </row>
     <row r="17">
@@ -1294,7 +1294,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2.022488050955991</v>
+        <v>1.364988858872664</v>
       </c>
     </row>
     <row r="18">
@@ -1302,7 +1302,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2.020655188295156</v>
+        <v>1.17386707108007</v>
       </c>
     </row>
     <row r="19">
@@ -1310,7 +1310,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2.018574058022685</v>
+        <v>1.002654426933297</v>
       </c>
     </row>
     <row r="20">
@@ -1318,7 +1318,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>2.01685703682148</v>
+        <v>0.8560020491517576</v>
       </c>
     </row>
     <row r="21">
@@ -1326,7 +1326,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>2.014560033695699</v>
+        <v>0.7280130570440712</v>
       </c>
     </row>
     <row r="22">
@@ -1334,7 +1334,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>2.012129125126024</v>
+        <v>0.6181056038693661</v>
       </c>
     </row>
     <row r="23">
@@ -1342,7 +1342,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>2.009980452523145</v>
+        <v>0.5259914720464036</v>
       </c>
     </row>
     <row r="24">
@@ -1350,7 +1350,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>2.007643280616806</v>
+        <v>0.4410233651521801</v>
       </c>
     </row>
     <row r="25">
@@ -1358,7 +1358,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>2.006166369635138</v>
+        <v>0.3760588320603483</v>
       </c>
     </row>
     <row r="26">
@@ -1366,7 +1366,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>2.001876665841754</v>
+        <v>0.3237219416673396</v>
       </c>
     </row>
     <row r="27">
@@ -1374,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.999107698231035</v>
+        <v>0.2775123782017636</v>
       </c>
     </row>
     <row r="28">
@@ -1382,7 +1382,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.996757143270779</v>
+        <v>0.2452920692585909</v>
       </c>
     </row>
     <row r="29">
@@ -1390,7 +1390,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.993817907629832</v>
+        <v>0.22056043282543</v>
       </c>
     </row>
     <row r="30">
@@ -1398,7 +1398,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.990100320750593</v>
+        <v>0.2001411085484042</v>
       </c>
     </row>
     <row r="31">
@@ -1406,7 +1406,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.985726624584774</v>
+        <v>0.1852721036943026</v>
       </c>
     </row>
     <row r="32">
@@ -1414,7 +1414,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.980629999040703</v>
+        <v>0.1743125006828568</v>
       </c>
     </row>
     <row r="33">
@@ -1422,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.974067832573625</v>
+        <v>0.1661867157694148</v>
       </c>
     </row>
     <row r="34">
@@ -1430,7 +1430,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.967297881334496</v>
+        <v>0.1592715530699424</v>
       </c>
     </row>
     <row r="35">
@@ -1438,7 +1438,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.960475365641328</v>
+        <v>0.1555651377921346</v>
       </c>
     </row>
     <row r="36">
@@ -1446,7 +1446,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.953221555230522</v>
+        <v>0.1527220723497398</v>
       </c>
     </row>
     <row r="37">
@@ -1454,7 +1454,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.943765354402497</v>
+        <v>0.1501037722987656</v>
       </c>
     </row>
     <row r="38">
@@ -1462,7 +1462,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.932200845261707</v>
+        <v>0.1490234554985705</v>
       </c>
     </row>
     <row r="39">
@@ -1470,7 +1470,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.920844879722508</v>
+        <v>0.1491726689312063</v>
       </c>
     </row>
     <row r="40">
@@ -1478,7 +1478,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.908683849055294</v>
+        <v>0.1472994254605554</v>
       </c>
     </row>
     <row r="41">
@@ -1486,7 +1486,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.895596800360764</v>
+        <v>0.1471230064210838</v>
       </c>
     </row>
     <row r="42">
@@ -1494,7 +1494,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.882787617245945</v>
+        <v>0.1473159898697378</v>
       </c>
     </row>
     <row r="43">
@@ -1502,7 +1502,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.86539855554017</v>
+        <v>0.1467969991653997</v>
       </c>
     </row>
     <row r="44">
@@ -1510,7 +1510,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.839507701985192</v>
+        <v>0.1467841704526569</v>
       </c>
     </row>
     <row r="45">
@@ -1518,7 +1518,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.805515182076332</v>
+        <v>0.1467322350663729</v>
       </c>
     </row>
     <row r="46">
@@ -1526,7 +1526,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.750677863034144</v>
+        <v>0.1466919191647262</v>
       </c>
     </row>
     <row r="47">
@@ -1534,7 +1534,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.674451464893047</v>
+        <v>0.1474109590225849</v>
       </c>
     </row>
     <row r="48">
@@ -1542,7 +1542,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.577167106966706</v>
+        <v>0.1462639103289659</v>
       </c>
     </row>
     <row r="49">
@@ -1550,7 +1550,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.491245391787422</v>
+        <v>0.1464776927695435</v>
       </c>
     </row>
     <row r="50">
@@ -1558,7 +1558,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.406207952930421</v>
+        <v>0.1468729016478779</v>
       </c>
     </row>
     <row r="51">
@@ -1566,7 +1566,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.323742536140126</v>
+        <v>0.1465857790595548</v>
       </c>
     </row>
     <row r="52">
@@ -1574,7 +1574,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>1.244845635216503</v>
+        <v>0.1479353378884886</v>
       </c>
     </row>
     <row r="53">
@@ -1582,7 +1582,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>1.169666549001713</v>
+        <v>0.1468191327208141</v>
       </c>
     </row>
     <row r="54">
@@ -1590,7 +1590,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1.096436987472264</v>
+        <v>0.1473333046407513</v>
       </c>
     </row>
     <row r="55">
@@ -1598,7 +1598,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1.023872981713455</v>
+        <v>0.1464565059854001</v>
       </c>
     </row>
     <row r="56">
@@ -1606,559 +1606,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.9528810470311114</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="n">
-        <v>0.8851839133617351</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="n">
-        <v>0.8213215752333842</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="n">
-        <v>0.7605389579435331</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="n">
-        <v>0.7035225274289092</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>0.6496564828533805</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="n">
-        <v>0.5992814201597024</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>0.5493256835154093</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>0.5053351495463982</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>0.4637391726882757</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>0.4263260531886313</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="n">
-        <v>0.3915795108360724</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="n">
-        <v>0.3613606412536073</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="n">
-        <v>0.3329349896855688</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>0.3070279730313752</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="n">
-        <v>0.2843356671222628</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="n">
-        <v>0.2638774211940523</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="n">
-        <v>0.2454336562709319</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="n">
-        <v>0.2302628421691652</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="n">
-        <v>0.2175766179496581</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="n">
-        <v>0.2056833691061914</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="n">
-        <v>0.1953990458428319</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>0.1867778899892773</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>0.1805039495349088</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="n">
-        <v>0.1748436985493057</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="n">
-        <v>0.1702208957263749</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" t="n">
-        <v>0.1665005054294372</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B83" t="n">
-        <v>0.1627979591304972</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B84" t="n">
-        <v>0.1603630812174946</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B85" t="n">
-        <v>0.1579097334951051</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" t="n">
-        <v>0.1558932523311974</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" t="n">
-        <v>0.1544949370958175</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" t="n">
-        <v>0.1525638347736902</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" t="n">
-        <v>0.1519791997489431</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="n">
-        <v>0.150638629733933</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="n">
-        <v>0.1503286481696933</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="n">
-        <v>0.1490306610016593</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="n">
-        <v>0.1484622620959751</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="n">
-        <v>0.1484017266282783</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="n">
-        <v>0.1479766492940548</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="n">
-        <v>0.1487605632409255</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="n">
-        <v>0.1477182808011752</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="n">
-        <v>0.1477182366681203</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="n">
-        <v>0.1470572522812238</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="n">
-        <v>0.1473606286337859</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="n">
-        <v>0.1469736384362134</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="n">
-        <v>0.1468286854687693</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="n">
-        <v>0.1467757759848068</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="n">
-        <v>0.146505417901812</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="n">
-        <v>0.1470495004100348</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="n">
-        <v>0.1467140622248292</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="n">
-        <v>0.1465545676856357</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="n">
-        <v>0.1465791840502317</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="n">
-        <v>0.1464793458711077</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="n">
-        <v>0.1463907387596924</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="n">
-        <v>0.146419847899154</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="n">
-        <v>0.1465106749766821</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="n">
-        <v>0.1463445313824018</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="n">
-        <v>0.146390859635656</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="n">
-        <v>0.1463318921229013</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="n">
-        <v>0.1465284471969871</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="n">
-        <v>0.1462178475848806</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="B118" t="n">
-        <v>0.1470209403583821</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>117</v>
-      </c>
-      <c r="B119" t="n">
-        <v>0.1464323841655271</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="B120" t="n">
-        <v>0.1468650956568255</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>119</v>
-      </c>
-      <c r="B121" t="n">
-        <v>0.14623544522756</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B122" t="n">
-        <v>0.1464509735173233</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="n">
-        <v>0.1462181660554285</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B124" t="n">
-        <v>0.1470361553411657</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="B125" t="n">
-        <v>0.1463600775745707</v>
+        <v>0.1468030705243395</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.979684515652148</v>
+        <v>0.9799589253938324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>